<commit_message>
Fix exception file code
</commit_message>
<xml_diff>
--- a/codeV3/exceptions.xlsx
+++ b/codeV3/exceptions.xlsx
@@ -9,114 +9,159 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Jy1C7FJIBCd8A2o+o3Alz4LZ4fklDKap1uRUZ4cRIEg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="BV+VFrELLHN+NBSJ+lF3dX8kCLy5vR2s1tclHAbzurs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
-  <si>
-    <t>name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
+  <si>
+    <t>replacement</t>
+  </si>
+  <si>
+    <t>replace</t>
   </si>
   <si>
     <t>California Institute of Technology</t>
   </si>
   <si>
-    <t>Colorado State University-Fort Collins</t>
-  </si>
-  <si>
-    <t>CUNY Graduate School and University Center</t>
-  </si>
-  <si>
-    <t>Georgia Institute of Technology-Main Campus</t>
-  </si>
-  <si>
-    <t>Indiana University-Bloomington</t>
-  </si>
-  <si>
-    <t>Indiana University-Purdue University-Indianapolis</t>
-  </si>
-  <si>
-    <t>Kent State University at Kent</t>
-  </si>
-  <si>
-    <t>New Mexico State University-Main Campus</t>
-  </si>
-  <si>
-    <t>North Dakota State University-Main Campus</t>
+    <t>Colorado State University</t>
+  </si>
+  <si>
+    <t>CUNY</t>
+  </si>
+  <si>
+    <t>Georgia Institute of Technology</t>
+  </si>
+  <si>
+    <t>Indiana University</t>
+  </si>
+  <si>
+    <t>Kent State University</t>
+  </si>
+  <si>
+    <t>New Mexico State University</t>
+  </si>
+  <si>
+    <t>North Dakota State University</t>
+  </si>
+  <si>
+    <t>OSU</t>
   </si>
   <si>
     <t>Ohio State University-Main Campus</t>
   </si>
   <si>
-    <t>Ohio University-Main Campus</t>
-  </si>
-  <si>
-    <t>Purdue University-Main Campus</t>
-  </si>
-  <si>
-    <t>Rutgers University-New Brunswick</t>
-  </si>
-  <si>
-    <t>Southern Illinois University-Carbondale</t>
-  </si>
-  <si>
-    <t>Texas A &amp; M University-College Station</t>
-  </si>
-  <si>
-    <t>The University of Tennessee Health Science Center</t>
-  </si>
-  <si>
-    <t>The University of Tennessee-Knoxville</t>
-  </si>
-  <si>
-    <t>The University of Texas Health Science Center at San Antonio</t>
+    <t>Ohio University</t>
+  </si>
+  <si>
+    <t>Purdue University</t>
+  </si>
+  <si>
+    <t>Rutgers University</t>
+  </si>
+  <si>
+    <t>Southern Illinois University</t>
+  </si>
+  <si>
+    <t>TX A&amp;M</t>
+  </si>
+  <si>
+    <t>Texas A &amp; M University</t>
+  </si>
+  <si>
+    <t>The University of Tennessee</t>
+  </si>
+  <si>
+    <t>U TX Austin</t>
+  </si>
+  <si>
+    <t>The University of Texas</t>
+  </si>
+  <si>
+    <t>UCB</t>
   </si>
   <si>
     <t>University of California-Berkeley</t>
   </si>
   <si>
+    <t>UCD</t>
+  </si>
+  <si>
     <t>University of California-Davis</t>
   </si>
   <si>
+    <t>UCI</t>
+  </si>
+  <si>
     <t>University of California-Irvine</t>
   </si>
   <si>
+    <t>UCLA</t>
+  </si>
+  <si>
     <t>University of California-Los Angeles</t>
   </si>
   <si>
+    <t>UCM</t>
+  </si>
+  <si>
     <t>University of California-Merced</t>
   </si>
   <si>
+    <t>UCR</t>
+  </si>
+  <si>
     <t>University of California-Riverside</t>
   </si>
   <si>
+    <t>UCSD</t>
+  </si>
+  <si>
     <t>University of California-San Diego</t>
   </si>
   <si>
+    <t>UCSF</t>
+  </si>
+  <si>
     <t>University of California-San Francisco</t>
   </si>
   <si>
     <t>University of California-Santa Barbara</t>
   </si>
   <si>
+    <t>UCSC</t>
+  </si>
+  <si>
     <t>University of California-Santa Cruz</t>
   </si>
   <si>
-    <t>University of Colorado Denver/Anschutz Medical Campus</t>
+    <t>University of Colorado Denver</t>
+  </si>
+  <si>
+    <t>UIUC</t>
   </si>
   <si>
     <t>University of Illinois Urbana-Champaign</t>
   </si>
   <si>
+    <t>UMBC</t>
+  </si>
+  <si>
     <t>University of Maryland-Baltimore County</t>
   </si>
   <si>
+    <t>UMCP</t>
+  </si>
+  <si>
     <t>University of Maryland-College Park</t>
   </si>
   <si>
+    <t>UMass</t>
+  </si>
+  <si>
     <t>University of Massachusetts-Amherst</t>
   </si>
   <si>
@@ -126,55 +171,79 @@
     <t>University of Massachusetts-Lowell</t>
   </si>
   <si>
-    <t>University of Michigan-Ann Arbor</t>
+    <t>University of Michigan</t>
+  </si>
+  <si>
+    <t>U MN Twin Cities</t>
   </si>
   <si>
     <t>University of Minnesota-Twin Cities</t>
   </si>
   <si>
+    <t>U MO</t>
+  </si>
+  <si>
     <t>University of Missouri-Columbia</t>
   </si>
   <si>
-    <t>University of Missouri-Kansas City</t>
+    <t>U NE Omaha</t>
   </si>
   <si>
     <t>University of Nebraska Medical Center</t>
   </si>
   <si>
+    <t>U NE Lincoln</t>
+  </si>
+  <si>
     <t>University of Nebraska-Lincoln</t>
   </si>
   <si>
+    <t>U NV</t>
+  </si>
+  <si>
     <t>University of Nevada-Las Vegas</t>
   </si>
   <si>
     <t>University of Nevada-Reno</t>
   </si>
   <si>
-    <t>University of New Hampshire-Main Campus</t>
-  </si>
-  <si>
-    <t>University of New Mexico-Main Campus</t>
-  </si>
-  <si>
-    <t>University of Oklahoma-Norman Campus</t>
-  </si>
-  <si>
-    <t>University of Pittsburgh-Pittsburgh Campus</t>
-  </si>
-  <si>
-    <t>University of South Carolina-Columbia</t>
-  </si>
-  <si>
-    <t>University of Virginia-Main Campus</t>
-  </si>
-  <si>
-    <t>University of Washington-Seattle Campus</t>
+    <t>University of New Hampshire</t>
+  </si>
+  <si>
+    <t>University of New Mexico</t>
+  </si>
+  <si>
+    <t>U OK Norman</t>
+  </si>
+  <si>
+    <t>University of Oklahoma</t>
+  </si>
+  <si>
+    <t>University of Pittsburgh</t>
+  </si>
+  <si>
+    <t>University of South Carolina</t>
+  </si>
+  <si>
+    <t>University of Virginia</t>
+  </si>
+  <si>
+    <t>University of Washington</t>
+  </si>
+  <si>
+    <t>U WI Madison</t>
   </si>
   <si>
     <t>University of Wisconsin-Madison</t>
   </si>
   <si>
+    <t>U WI Milwaukee</t>
+  </si>
+  <si>
     <t>University of Wisconsin-Milwaukee</t>
+  </si>
+  <si>
+    <t>Cornell U</t>
   </si>
   <si>
     <t>Weill Medical College of Cornell University</t>
@@ -184,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -201,6 +270,10 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -224,6 +297,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -440,279 +519,366 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="10.56"/>
+    <col customWidth="1" min="1" max="1" width="50.89"/>
+    <col customWidth="1" min="2" max="26" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
+      <c r="A9" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
+      <c r="A11" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
+      <c r="A12" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
+      <c r="A13" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
+      <c r="A14" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
+      <c r="A16" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
+      <c r="A17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
+      <c r="A21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
+      <c r="A23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
+      <c r="A24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
+      <c r="A25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
+      <c r="A27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
+      <c r="A28" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
+      <c r="A29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
+      <c r="A30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
+      <c r="A31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
+      <c r="A32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>32</v>
+      <c r="A33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>33</v>
+      <c r="A34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>34</v>
+      <c r="A35" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>35</v>
+      <c r="A36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>36</v>
+      <c r="A37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="2" t="s">
-        <v>37</v>
+      <c r="A38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>38</v>
+      <c r="A39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>39</v>
+      <c r="A40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="2" t="s">
-        <v>40</v>
+      <c r="A41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="2" t="s">
-        <v>41</v>
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>42</v>
+      <c r="A43" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>43</v>
+      <c r="A44" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>44</v>
+      <c r="A45" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>45</v>
+      <c r="A46" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="2" t="s">
-        <v>46</v>
+      <c r="A47" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="2" t="s">
-        <v>47</v>
+      <c r="A48" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>48</v>
+      <c r="A49" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2" t="s">
-        <v>49</v>
+      <c r="A50" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2" t="s">
-        <v>50</v>
+      <c r="A51" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
+      <c r="A52" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1"/>
@@ -1658,8 +1824,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>